<commit_message>
Switch to using Excel for input
</commit_message>
<xml_diff>
--- a/Input_Scoreboard_Data.xlsx
+++ b/Input_Scoreboard_Data.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Jeremy\Documents\RW\Masters_Classes\Freelancer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacea\OneDrive\Documents\GitHub\Squid-Game-Scores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F2DBEF0-0570-432A-BFCC-A73421C604B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4E0998-1637-4360-9A3A-B7CF2A64E03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27255" yWindow="3540" windowWidth="21600" windowHeight="11385" xr2:uid="{0BA77F5B-3010-4EA6-9FC4-6D5980AA6358}"/>
+    <workbookView xWindow="-26970" yWindow="2970" windowWidth="21600" windowHeight="11385" xr2:uid="{0BA77F5B-3010-4EA6-9FC4-6D5980AA6358}"/>
   </bookViews>
   <sheets>
-    <sheet name="notes" sheetId="4" r:id="rId1"/>
-    <sheet name="results-1" sheetId="1" r:id="rId2"/>
-    <sheet name="results-2" sheetId="2" r:id="rId3"/>
-    <sheet name="results-3" sheetId="3" r:id="rId4"/>
+    <sheet name="results-1" sheetId="1" r:id="rId1"/>
+    <sheet name="results-2" sheetId="2" r:id="rId2"/>
+    <sheet name="results-3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="80">
   <si>
     <t>Result</t>
   </si>
@@ -279,12 +278,6 @@
   </si>
   <si>
     <t>Opp-3:Splatana-Stamper-Nouveau_844_12_5_5_1,Opp-1:Order-Stringer-Replica_787_6_4_5_4,Opp-4:Splat-Roller_664_7_3_6_2,Opp-2:Splat-Dualies_763_7_1_7_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weapon names based on </t>
-  </si>
-  <si>
-    <t>https://splatoonwiki.org/wiki/List_of_main_weapons_in_Splatoon_3</t>
   </si>
 </sst>
 </file>
@@ -655,34 +648,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EAC10B-B6AD-43C4-84A9-21CCED78023B}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D3287B-3C3E-4535-AB5F-7DAD863B5995}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD84BB4-C588-4009-A061-81CDF7894EA7}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -1158,7 +1128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4763CA1D-318C-4A08-B8B8-E85AC66A8AE0}">
   <dimension ref="A1:M7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Switch to using only first row for Date and Opponent*
*The values in the first row for Date and Opponent_Team are now used to set the values for all other rows, so it's unnecessary to manually specify those for every row
</commit_message>
<xml_diff>
--- a/Input_Scoreboard_Data.xlsx
+++ b/Input_Scoreboard_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacea\OneDrive\Documents\GitHub\Squid-Game-Scores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4E0998-1637-4360-9A3A-B7CF2A64E03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8C21DD-CB63-42F3-8DEC-A6AB704D7AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26970" yWindow="2970" windowWidth="21600" windowHeight="11385" xr2:uid="{0BA77F5B-3010-4EA6-9FC4-6D5980AA6358}"/>
+    <workbookView xWindow="-28920" yWindow="660" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0BA77F5B-3010-4EA6-9FC4-6D5980AA6358}"/>
   </bookViews>
   <sheets>
     <sheet name="results-1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="80">
   <si>
     <t>Result</t>
   </si>
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D3287B-3C3E-4535-AB5F-7DAD863B5995}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,12 +716,6 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
@@ -754,12 +748,6 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" t="s">
         <v>26</v>
       </c>
@@ -789,12 +777,6 @@
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
       <c r="E5" t="s">
         <v>30</v>
       </c>
@@ -824,12 +806,6 @@
       <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
@@ -855,12 +831,6 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
@@ -894,7 +864,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M7"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,12 +928,6 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
       <c r="E3" t="s">
         <v>46</v>
       </c>
@@ -996,12 +960,6 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
       <c r="E4" t="s">
         <v>50</v>
       </c>
@@ -1028,12 +986,6 @@
       <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>45</v>
-      </c>
       <c r="E5" t="s">
         <v>53</v>
       </c>
@@ -1063,12 +1015,6 @@
       <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
       <c r="E6" t="s">
         <v>56</v>
       </c>
@@ -1094,12 +1040,6 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
       </c>
       <c r="E7" t="s">
         <v>26</v>
@@ -1132,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4763CA1D-318C-4A08-B8B8-E85AC66A8AE0}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,12 +1137,6 @@
       <c r="A3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
       <c r="E3" t="s">
         <v>64</v>
       </c>
@@ -1235,12 +1169,6 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" t="s">
-        <v>63</v>
-      </c>
       <c r="E4" t="s">
         <v>67</v>
       </c>
@@ -1270,12 +1198,6 @@
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" t="s">
-        <v>63</v>
-      </c>
       <c r="E5" t="s">
         <v>70</v>
       </c>
@@ -1302,12 +1224,6 @@
       <c r="A6" t="s">
         <v>73</v>
       </c>
-      <c r="C6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
       <c r="E6" t="s">
         <v>74</v>
       </c>
@@ -1336,12 +1252,6 @@
       </c>
       <c r="B7" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
       </c>
       <c r="E7" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
Add test cases for 4v3 and 3v4*
*Add filter to weapons data to remove propagated empty rows
</commit_message>
<xml_diff>
--- a/Input_Scoreboard_Data.xlsx
+++ b/Input_Scoreboard_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacea\OneDrive\Documents\GitHub\Squid-Game-Scores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8C21DD-CB63-42F3-8DEC-A6AB704D7AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C91F2D-591C-4B11-A0AE-0901F3260909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="660" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0BA77F5B-3010-4EA6-9FC4-6D5980AA6358}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0BA77F5B-3010-4EA6-9FC4-6D5980AA6358}"/>
   </bookViews>
   <sheets>
     <sheet name="results-1" sheetId="1" r:id="rId1"/>
@@ -205,15 +205,9 @@
     <t>Player-1:Tentatek-Splattershot_2055_31_2_6_8,Player-3:Splatterscope_1280_9_8_3_6,Player-6:Painbrush_1226_8_3_10_5,Player-4:Splattershot-Jr_1283_4_1_13_3</t>
   </si>
   <si>
-    <t>Opp-4:Splattershot-Jr_1893_19_3_9_7,Opp-6:Neo-Splash-o-matic_1386_15_8_7_5,Opp-3:Nautilus-79_1141_5_2_11_4,Opp-1:Custom-Blaster_1164_11_5_11_4</t>
-  </si>
-  <si>
     <t>Eeltail-Alley</t>
   </si>
   <si>
-    <t>Player-1:Tentatek-Splattershot_953_12_1_3_2,Player-5:Hydra-Splatling_521_4_2_5_1,Player-4:Octo-Shot-Replica_621_2_1_4_1,Player-Two:Splash-o-matic_701_10_0_6_3</t>
-  </si>
-  <si>
     <t>Opp-5:Tri-Slosher-Nouveau_600_8_2_6_2,Opp-2:Splattershot_629_7_1_7_1,Opp-6:Splattershot_683_6_3_5_2,Opp-1:Rapid-Blaster-Deco_440_5_2_6_0</t>
   </si>
   <si>
@@ -278,6 +272,12 @@
   </si>
   <si>
     <t>Opp-3:Splatana-Stamper-Nouveau_844_12_5_5_1,Opp-1:Order-Stringer-Replica_787_6_4_5_4,Opp-4:Splat-Roller_664_7_3_6_2,Opp-2:Splat-Dualies_763_7_1_7_1</t>
+  </si>
+  <si>
+    <t>Player-1:Tentatek-Splattershot_953_12_1_3_2,Player-5:Hydra-Splatling_521_4_2_5_1,Player-Two:Splash-o-matic_701_10_0_6_3</t>
+  </si>
+  <si>
+    <t>Opp-4:Splattershot-Jr_1893_19_3_9_7,Opp-3:Nautilus-79_1141_5_2_11_4,Opp-1:Custom-Blaster_1164_11_5_11_4</t>
   </si>
 </sst>
 </file>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD84BB4-C588-4009-A061-81CDF7894EA7}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +999,7 @@
         <v>54</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="J5">
         <v>3</v>
@@ -1016,7 +1016,7 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
@@ -1025,10 +1025,10 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J6">
         <v>4</v>
@@ -1051,10 +1051,10 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J7">
         <v>5</v>
@@ -1072,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4763CA1D-318C-4A08-B8B8-E85AC66A8AE0}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,13 +1121,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
@@ -1138,7 +1138,7 @@
         <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -1147,10 +1147,10 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1170,7 +1170,7 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
@@ -1179,10 +1179,10 @@
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -1199,7 +1199,7 @@
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
         <v>31</v>
@@ -1208,10 +1208,10 @@
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J5">
         <v>3</v>
@@ -1222,10 +1222,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
@@ -1234,10 +1234,10 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J6">
         <v>4</v>
@@ -1254,7 +1254,7 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F7" t="s">
         <v>40</v>
@@ -1263,10 +1263,10 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J7">
         <v>5</v>

</xml_diff>

<commit_message>
Move changelog to external file and update it
</commit_message>
<xml_diff>
--- a/Input_Scoreboard_Data.xlsx
+++ b/Input_Scoreboard_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacea\OneDrive\Documents\GitHub\Squid-Game-Scores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C91F2D-591C-4B11-A0AE-0901F3260909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283C7272-B84B-40A3-8609-79C3AF4B971A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0BA77F5B-3010-4EA6-9FC4-6D5980AA6358}"/>
+    <workbookView xWindow="-28920" yWindow="660" windowWidth="29040" windowHeight="15840" xr2:uid="{0BA77F5B-3010-4EA6-9FC4-6D5980AA6358}"/>
   </bookViews>
   <sheets>
     <sheet name="results-1" sheetId="1" r:id="rId1"/>
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D3287B-3C3E-4535-AB5F-7DAD863B5995}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD84BB4-C588-4009-A061-81CDF7894EA7}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>

</xml_diff>